<commit_message>
Fixed distance rounding bug into integer
</commit_message>
<xml_diff>
--- a/data/dataProfile3D.xlsx
+++ b/data/dataProfile3D.xlsx
@@ -21,10 +21,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="17">
   <x:si>
-    <x:t>[3 6 1]</x:t>
+    <x:t>[4 5 6]</x:t>
   </x:si>
   <x:si>
-    <x:t>[8 5 4]</x:t>
+    <x:t>[7 7 3]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[6 2 3]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[5 5 5]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[6 3 3]</x:t>
   </x:si>
   <x:si>
     <x:t>[6 6 2]</x:t>
@@ -33,31 +42,19 @@
     <x:t>[4 4 5]</x:t>
   </x:si>
   <x:si>
-    <x:t>[7 7 3]</x:t>
+    <x:t>[2 8 4]</x:t>
   </x:si>
   <x:si>
-    <x:t>[4 5 6]</x:t>
+    <x:t>[8 5 4]</x:t>
   </x:si>
   <x:si>
-    <x:t>[6 3 3]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[5 5 5]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[7 5 6]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[6 2 3]</x:t>
+    <x:t>[3 6 1]</x:t>
   </x:si>
   <x:si>
     <x:t>[6 5 4]</x:t>
   </x:si>
   <x:si>
-    <x:t>[2 8 4]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[16 6 10]</x:t>
+    <x:t>[7 5 6]</x:t>
   </x:si>
   <x:si>
     <x:t>[6 3 10]</x:t>
@@ -66,10 +63,13 @@
     <x:t>[13 6 9]</x:t>
   </x:si>
   <x:si>
-    <x:t>[6 5 10]</x:t>
+    <x:t>[16 6 10]</x:t>
   </x:si>
   <x:si>
     <x:t>[3 12 1]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[6 5 10]</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -801,7 +801,7 @@
   <x:dimension ref="A1:O60"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="A1" activeCellId="0" sqref="A1:A1"/>
+      <x:selection activeCell="G4" activeCellId="0" sqref="G4:G4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
@@ -814,43 +814,43 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C1" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E1">
+        <x:v>1.41421356237309</x:v>
+      </x:c>
+      <x:c r="F1">
+        <x:v>1870101</x:v>
+      </x:c>
+      <x:c r="G1">
+        <x:v>69401</x:v>
+      </x:c>
+      <x:c r="H1" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E1">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F1">
-        <x:v>2598998</x:v>
-      </x:c>
-      <x:c r="G1">
-        <x:v>116200</x:v>
-      </x:c>
-      <x:c r="H1" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="I1">
-        <x:v>3</x:v>
+        <x:v>3.3166247903553998</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>3282300</x:v>
+        <x:v>3039499</x:v>
       </x:c>
       <x:c r="K1">
-        <x:v>121600</x:v>
+        <x:v>76200</x:v>
       </x:c>
       <x:c r="L1" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="M1">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N1">
-        <x:v>3282300</x:v>
+        <x:v>3039499</x:v>
       </x:c>
       <x:c r="O1">
-        <x:v>107200</x:v>
+        <x:v>258399</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:15">
@@ -861,43 +861,43 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C2" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E2">
+        <x:v>1.41421356237309</x:v>
+      </x:c>
+      <x:c r="F2">
+        <x:v>22901</x:v>
+      </x:c>
+      <x:c r="G2">
+        <x:v>17200</x:v>
+      </x:c>
+      <x:c r="H2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E2">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F2">
-        <x:v>17800</x:v>
-      </x:c>
-      <x:c r="G2">
-        <x:v>18201</x:v>
-      </x:c>
-      <x:c r="H2" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="I2">
-        <x:v>3</x:v>
+        <x:v>3.3166247903553998</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>213500</x:v>
+        <x:v>661600</x:v>
       </x:c>
       <x:c r="K2">
-        <x:v>19299</x:v>
+        <x:v>15900</x:v>
       </x:c>
       <x:c r="L2" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="M2">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N2">
-        <x:v>213500</x:v>
+        <x:v>661600</x:v>
       </x:c>
       <x:c r="O2">
-        <x:v>37000</x:v>
+        <x:v>32400</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:15">
@@ -908,43 +908,43 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C3" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D3" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E3">
+        <x:v>1.41421356237309</x:v>
+      </x:c>
+      <x:c r="F3">
+        <x:v>18900</x:v>
+      </x:c>
+      <x:c r="G3">
+        <x:v>18400</x:v>
+      </x:c>
+      <x:c r="H3" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E3">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F3">
-        <x:v>19202</x:v>
-      </x:c>
-      <x:c r="G3">
-        <x:v>20400</x:v>
-      </x:c>
-      <x:c r="H3" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="I3">
-        <x:v>3</x:v>
+        <x:v>3.3166247903553998</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>481300</x:v>
+        <x:v>250700</x:v>
       </x:c>
       <x:c r="K3">
-        <x:v>18299</x:v>
+        <x:v>18099</x:v>
       </x:c>
       <x:c r="L3" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="M3">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N3">
-        <x:v>481300</x:v>
+        <x:v>250700</x:v>
       </x:c>
       <x:c r="O3">
-        <x:v>359300</x:v>
+        <x:v>325401</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:15">
@@ -955,43 +955,43 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C4" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E4">
+        <x:v>1.41421356237309</x:v>
+      </x:c>
+      <x:c r="F4">
+        <x:v>15899</x:v>
+      </x:c>
+      <x:c r="G4">
+        <x:v>17999</x:v>
+      </x:c>
+      <x:c r="H4" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E4">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F4">
-        <x:v>11398</x:v>
-      </x:c>
-      <x:c r="G4">
-        <x:v>13201</x:v>
-      </x:c>
-      <x:c r="H4" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="I4">
-        <x:v>3</x:v>
+        <x:v>3.3166247903553998</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>206000</x:v>
+        <x:v>250200</x:v>
       </x:c>
       <x:c r="K4">
-        <x:v>15900</x:v>
+        <x:v>17100</x:v>
       </x:c>
       <x:c r="L4" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="M4">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N4">
-        <x:v>206000</x:v>
+        <x:v>250200</x:v>
       </x:c>
       <x:c r="O4">
-        <x:v>28400</x:v>
+        <x:v>27399</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:15">
@@ -1002,43 +1002,43 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C5" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D5" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E5">
+        <x:v>1.41421356237309</x:v>
+      </x:c>
+      <x:c r="F5">
+        <x:v>13399</x:v>
+      </x:c>
+      <x:c r="G5">
+        <x:v>13900</x:v>
+      </x:c>
+      <x:c r="H5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="E5">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F5">
-        <x:v>14300</x:v>
-      </x:c>
-      <x:c r="G5">
-        <x:v>14200</x:v>
-      </x:c>
-      <x:c r="H5" t="s">
-        <x:v>2</x:v>
-      </x:c>
       <x:c r="I5">
-        <x:v>3</x:v>
+        <x:v>3.3166247903553998</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>222201</x:v>
+        <x:v>208300</x:v>
       </x:c>
       <x:c r="K5">
-        <x:v>15900</x:v>
+        <x:v>16600</x:v>
       </x:c>
       <x:c r="L5" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="M5">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N5">
-        <x:v>222201</x:v>
+        <x:v>208300</x:v>
       </x:c>
       <x:c r="O5">
-        <x:v>31100</x:v>
+        <x:v>33900</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:15">
@@ -1049,43 +1049,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C6" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D6" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>33503</x:v>
+        <x:v>110397</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>38100</x:v>
+        <x:v>43000</x:v>
       </x:c>
       <x:c r="H6" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>566901</x:v>
+        <x:v>712800</x:v>
       </x:c>
       <x:c r="K6">
-        <x:v>14200</x:v>
+        <x:v>20800</x:v>
       </x:c>
       <x:c r="L6" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="M6">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="N6">
-        <x:v>566901</x:v>
+        <x:v>712800</x:v>
       </x:c>
       <x:c r="O6">
-        <x:v>215500</x:v>
+        <x:v>504400</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:15">
@@ -1096,43 +1096,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C7" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D7" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>27498</x:v>
+        <x:v>26400</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>33100</x:v>
+        <x:v>33801</x:v>
       </x:c>
       <x:c r="H7" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>627700</x:v>
+        <x:v>442800</x:v>
       </x:c>
       <x:c r="K7">
-        <x:v>21700</x:v>
+        <x:v>20501</x:v>
       </x:c>
       <x:c r="L7" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="M7">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="N7">
-        <x:v>627700</x:v>
+        <x:v>442800</x:v>
       </x:c>
       <x:c r="O7">
-        <x:v>312000</x:v>
+        <x:v>183000</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:15">
@@ -1143,43 +1143,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C8" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D8" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>1100099</x:v>
+        <x:v>1323600</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>50601</x:v>
+        <x:v>68500</x:v>
       </x:c>
       <x:c r="H8" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>514699</x:v>
+        <x:v>513401</x:v>
       </x:c>
       <x:c r="K8">
-        <x:v>19201</x:v>
+        <x:v>20599</x:v>
       </x:c>
       <x:c r="L8" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="M8">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="N8">
-        <x:v>514699</x:v>
+        <x:v>513401</x:v>
       </x:c>
       <x:c r="O8">
-        <x:v>171399</x:v>
+        <x:v>539099</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:15">
@@ -1190,43 +1190,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C9" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D9" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>30101</x:v>
+        <x:v>38200</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>44299</x:v>
+        <x:v>71300</x:v>
       </x:c>
       <x:c r="H9" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>1390800</x:v>
+        <x:v>566100</x:v>
       </x:c>
       <x:c r="K9">
-        <x:v>21700</x:v>
+        <x:v>21000</x:v>
       </x:c>
       <x:c r="L9" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="M9">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="N9">
-        <x:v>1390800</x:v>
+        <x:v>566100</x:v>
       </x:c>
       <x:c r="O9">
-        <x:v>158101</x:v>
+        <x:v>91300</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:15">
@@ -1237,43 +1237,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C10" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D10" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>35299</x:v>
+        <x:v>39202</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>32301</x:v>
+        <x:v>35000</x:v>
       </x:c>
       <x:c r="H10" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>313400</x:v>
+        <x:v>688600</x:v>
       </x:c>
       <x:c r="K10">
-        <x:v>21700</x:v>
+        <x:v>22100</x:v>
       </x:c>
       <x:c r="L10" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="M10">
-        <x:v>2</x:v>
+        <x:v>2.2360679774997898</x:v>
       </x:c>
       <x:c r="N10">
-        <x:v>313400</x:v>
+        <x:v>688600</x:v>
       </x:c>
       <x:c r="O10">
-        <x:v>165699</x:v>
+        <x:v>174499</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:15">
@@ -1284,43 +1284,43 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C11" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D11" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>22600</x:v>
+        <x:v>19700</x:v>
       </x:c>
       <x:c r="G11">
         <x:v>32400</x:v>
       </x:c>
       <x:c r="H11" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>12</x:v>
+        <x:v>12.1243556529821</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>328800</x:v>
+        <x:v>324900</x:v>
       </x:c>
       <x:c r="K11">
-        <x:v>20701</x:v>
+        <x:v>20300</x:v>
       </x:c>
       <x:c r="L11" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M11">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="N11">
-        <x:v>328800</x:v>
+        <x:v>324900</x:v>
       </x:c>
       <x:c r="O11">
-        <x:v>160300</x:v>
+        <x:v>112199</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:15">
@@ -1331,43 +1331,43 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C12" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D12" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>32899</x:v>
+        <x:v>32500</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>46100</x:v>
+        <x:v>47400</x:v>
       </x:c>
       <x:c r="H12" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>12</x:v>
+        <x:v>12.1243556529821</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>1177200</x:v>
+        <x:v>823300</x:v>
       </x:c>
       <x:c r="K12">
-        <x:v>22899</x:v>
+        <x:v>23900</x:v>
       </x:c>
       <x:c r="L12" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M12">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="N12">
-        <x:v>1177200</x:v>
+        <x:v>823300</x:v>
       </x:c>
       <x:c r="O12">
-        <x:v>123400</x:v>
+        <x:v>70300</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:15">
@@ -1378,43 +1378,43 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C13" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D13" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>65702</x:v>
+        <x:v>36900</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>517000</x:v>
+        <x:v>96600</x:v>
       </x:c>
       <x:c r="H13" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>12</x:v>
+        <x:v>12.1243556529821</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>416200</x:v>
+        <x:v>693000</x:v>
       </x:c>
       <x:c r="K13">
-        <x:v>21399</x:v>
+        <x:v>27500</x:v>
       </x:c>
       <x:c r="L13" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M13">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="N13">
-        <x:v>416200</x:v>
+        <x:v>693000</x:v>
       </x:c>
       <x:c r="O13">
-        <x:v>82699</x:v>
+        <x:v>110400</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:15">
@@ -1425,43 +1425,43 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C14" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D14" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>33200</x:v>
+        <x:v>37200</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>48800</x:v>
+        <x:v>51799</x:v>
       </x:c>
       <x:c r="H14" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>12</x:v>
+        <x:v>12.1243556529821</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>1155500</x:v>
+        <x:v>354600</x:v>
       </x:c>
       <x:c r="K14">
-        <x:v>20600</x:v>
+        <x:v>15400</x:v>
       </x:c>
       <x:c r="L14" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M14">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="N14">
-        <x:v>1155500</x:v>
+        <x:v>354600</x:v>
       </x:c>
       <x:c r="O14">
-        <x:v>496200</x:v>
+        <x:v>166799</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:15">
@@ -1472,43 +1472,43 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="C15" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D15" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>17898</x:v>
+        <x:v>19700</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>31400</x:v>
+        <x:v>31900</x:v>
       </x:c>
       <x:c r="H15" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>12</x:v>
+        <x:v>12.1243556529821</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>299000</x:v>
+        <x:v>332100</x:v>
       </x:c>
       <x:c r="K15">
-        <x:v>7600</x:v>
+        <x:v>9100</x:v>
       </x:c>
       <x:c r="L15" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="M15">
-        <x:v>3</x:v>
+        <x:v>3.74165738677394</x:v>
       </x:c>
       <x:c r="N15">
-        <x:v>299000</x:v>
+        <x:v>332100</x:v>
       </x:c>
       <x:c r="O15">
-        <x:v>48499</x:v>
+        <x:v>42000</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:15">
@@ -1519,43 +1519,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C16" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D16" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E16">
+        <x:v>5.4772255750516603</x:v>
+      </x:c>
+      <x:c r="F16">
+        <x:v>12700</x:v>
+      </x:c>
+      <x:c r="G16">
+        <x:v>41699</x:v>
+      </x:c>
+      <x:c r="H16" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E16">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F16">
-        <x:v>26900</x:v>
-      </x:c>
-      <x:c r="G16">
-        <x:v>39900</x:v>
-      </x:c>
-      <x:c r="H16" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="I16">
         <x:v>9</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>951801</x:v>
+        <x:v>625500</x:v>
       </x:c>
       <x:c r="K16">
-        <x:v>13400</x:v>
+        <x:v>12900</x:v>
       </x:c>
       <x:c r="L16" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M16">
-        <x:v>5</x:v>
+        <x:v>5.4772255750516603</x:v>
       </x:c>
       <x:c r="N16">
-        <x:v>951801</x:v>
+        <x:v>625500</x:v>
       </x:c>
       <x:c r="O16">
-        <x:v>13100</x:v>
+        <x:v>10001</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:15">
@@ -1566,43 +1566,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C17" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D17" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E17">
+        <x:v>5.4772255750516603</x:v>
+      </x:c>
+      <x:c r="F17">
+        <x:v>18101</x:v>
+      </x:c>
+      <x:c r="G17">
+        <x:v>64699</x:v>
+      </x:c>
+      <x:c r="H17" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E17">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F17">
-        <x:v>21600</x:v>
-      </x:c>
-      <x:c r="G17">
-        <x:v>97301</x:v>
-      </x:c>
-      <x:c r="H17" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="I17">
         <x:v>9</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>674700</x:v>
+        <x:v>1083900</x:v>
       </x:c>
       <x:c r="K17">
-        <x:v>8800</x:v>
+        <x:v>12800</x:v>
       </x:c>
       <x:c r="L17" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M17">
-        <x:v>5</x:v>
+        <x:v>5.4772255750516603</x:v>
       </x:c>
       <x:c r="N17">
-        <x:v>674700</x:v>
+        <x:v>1083900</x:v>
       </x:c>
       <x:c r="O17">
-        <x:v>9701</x:v>
+        <x:v>357999</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:15">
@@ -1613,43 +1613,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C18" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D18" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E18">
+        <x:v>5.4772255750516603</x:v>
+      </x:c>
+      <x:c r="F18">
+        <x:v>18501</x:v>
+      </x:c>
+      <x:c r="G18">
+        <x:v>21699</x:v>
+      </x:c>
+      <x:c r="H18" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E18">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F18">
-        <x:v>40098</x:v>
-      </x:c>
-      <x:c r="G18">
-        <x:v>19499</x:v>
-      </x:c>
-      <x:c r="H18" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="I18">
         <x:v>9</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>413900</x:v>
+        <x:v>345901</x:v>
       </x:c>
       <x:c r="K18">
-        <x:v>11900</x:v>
+        <x:v>17299</x:v>
       </x:c>
       <x:c r="L18" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M18">
-        <x:v>5</x:v>
+        <x:v>5.4772255750516603</x:v>
       </x:c>
       <x:c r="N18">
-        <x:v>413900</x:v>
+        <x:v>345901</x:v>
       </x:c>
       <x:c r="O18">
-        <x:v>11801</x:v>
+        <x:v>223900</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:15">
@@ -1660,43 +1660,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C19" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D19" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E19">
+        <x:v>5.4772255750516603</x:v>
+      </x:c>
+      <x:c r="F19">
+        <x:v>13602</x:v>
+      </x:c>
+      <x:c r="G19">
+        <x:v>17500</x:v>
+      </x:c>
+      <x:c r="H19" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E19">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F19">
-        <x:v>162000</x:v>
-      </x:c>
-      <x:c r="G19">
-        <x:v>24500</x:v>
-      </x:c>
-      <x:c r="H19" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="I19">
         <x:v>9</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>410100</x:v>
+        <x:v>500200</x:v>
       </x:c>
       <x:c r="K19">
-        <x:v>12400</x:v>
+        <x:v>14200</x:v>
       </x:c>
       <x:c r="L19" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M19">
-        <x:v>5</x:v>
+        <x:v>5.4772255750516603</x:v>
       </x:c>
       <x:c r="N19">
-        <x:v>410100</x:v>
+        <x:v>500200</x:v>
       </x:c>
       <x:c r="O19">
-        <x:v>10400</x:v>
+        <x:v>11001</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:15">
@@ -1707,43 +1707,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C20" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D20" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E20">
+        <x:v>5.4772255750516603</x:v>
+      </x:c>
+      <x:c r="F20">
+        <x:v>21797</x:v>
+      </x:c>
+      <x:c r="G20">
+        <x:v>29600</x:v>
+      </x:c>
+      <x:c r="H20" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E20">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="F20">
-        <x:v>73299</x:v>
-      </x:c>
-      <x:c r="G20">
-        <x:v>14200</x:v>
-      </x:c>
-      <x:c r="H20" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="I20">
         <x:v>9</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>1214699</x:v>
+        <x:v>681900</x:v>
       </x:c>
       <x:c r="K20">
-        <x:v>19900</x:v>
+        <x:v>15300</x:v>
       </x:c>
       <x:c r="L20" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M20">
-        <x:v>5</x:v>
+        <x:v>5.4772255750516603</x:v>
       </x:c>
       <x:c r="N20">
-        <x:v>1214699</x:v>
+        <x:v>681900</x:v>
       </x:c>
       <x:c r="O20">
-        <x:v>16300</x:v>
+        <x:v>234300</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:15">
@@ -1754,43 +1754,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C21" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D21" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E21">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F21">
-        <x:v>6101</x:v>
+        <x:v>6600</x:v>
       </x:c>
       <x:c r="G21">
-        <x:v>7801</x:v>
+        <x:v>8501</x:v>
       </x:c>
       <x:c r="H21" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="I21">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J21">
-        <x:v>161100</x:v>
+        <x:v>228900</x:v>
       </x:c>
       <x:c r="K21">
-        <x:v>15700</x:v>
+        <x:v>12101</x:v>
       </x:c>
       <x:c r="L21" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="M21">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N21">
-        <x:v>161100</x:v>
+        <x:v>228900</x:v>
       </x:c>
       <x:c r="O21">
-        <x:v>7999</x:v>
+        <x:v>6601</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:15">
@@ -1801,43 +1801,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C22" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D22" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E22">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F22">
-        <x:v>5899</x:v>
+        <x:v>12799</x:v>
       </x:c>
       <x:c r="G22">
-        <x:v>7600</x:v>
+        <x:v>11200</x:v>
       </x:c>
       <x:c r="H22" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="I22">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J22">
-        <x:v>120500</x:v>
+        <x:v>95601</x:v>
       </x:c>
       <x:c r="K22">
-        <x:v>12101</x:v>
+        <x:v>11000</x:v>
       </x:c>
       <x:c r="L22" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="M22">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N22">
-        <x:v>120500</x:v>
+        <x:v>95601</x:v>
       </x:c>
       <x:c r="O22">
-        <x:v>6000</x:v>
+        <x:v>6200</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:15">
@@ -1848,43 +1848,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C23" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D23" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E23">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F23">
-        <x:v>9099</x:v>
+        <x:v>9001</x:v>
       </x:c>
       <x:c r="G23">
-        <x:v>11000</x:v>
+        <x:v>9601</x:v>
       </x:c>
       <x:c r="H23" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="I23">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J23">
-        <x:v>77600</x:v>
+        <x:v>144900</x:v>
       </x:c>
       <x:c r="K23">
-        <x:v>11501</x:v>
+        <x:v>12700</x:v>
       </x:c>
       <x:c r="L23" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="M23">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N23">
-        <x:v>77600</x:v>
+        <x:v>144900</x:v>
       </x:c>
       <x:c r="O23">
-        <x:v>6000</x:v>
+        <x:v>6700</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:15">
@@ -1895,43 +1895,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C24" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D24" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E24">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F24">
-        <x:v>7001</x:v>
+        <x:v>10400</x:v>
       </x:c>
       <x:c r="G24">
-        <x:v>7300</x:v>
+        <x:v>11800</x:v>
       </x:c>
       <x:c r="H24" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="I24">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J24">
-        <x:v>179900</x:v>
+        <x:v>305500</x:v>
       </x:c>
       <x:c r="K24">
-        <x:v>12200</x:v>
+        <x:v>14400</x:v>
       </x:c>
       <x:c r="L24" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="M24">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N24">
-        <x:v>179900</x:v>
+        <x:v>305500</x:v>
       </x:c>
       <x:c r="O24">
-        <x:v>6399</x:v>
+        <x:v>7199</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:15">
@@ -1942,43 +1942,43 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C25" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D25" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E25">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F25">
-        <x:v>6900</x:v>
+        <x:v>6401</x:v>
       </x:c>
       <x:c r="G25">
-        <x:v>7800</x:v>
+        <x:v>7801</x:v>
       </x:c>
       <x:c r="H25" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="I25">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J25">
-        <x:v>118400</x:v>
+        <x:v>81899</x:v>
       </x:c>
       <x:c r="K25">
-        <x:v>11900</x:v>
+        <x:v>16500</x:v>
       </x:c>
       <x:c r="L25" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="M25">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N25">
-        <x:v>118400</x:v>
+        <x:v>81899</x:v>
       </x:c>
       <x:c r="O25">
-        <x:v>6399</x:v>
+        <x:v>5701</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:15">
@@ -1989,43 +1989,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C26" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D26" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E26">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F26">
-        <x:v>18501</x:v>
+        <x:v>16399</x:v>
       </x:c>
       <x:c r="G26">
-        <x:v>18500</x:v>
+        <x:v>18000</x:v>
       </x:c>
       <x:c r="H26" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I26">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J26">
-        <x:v>421000</x:v>
+        <x:v>236200</x:v>
       </x:c>
       <x:c r="K26">
-        <x:v>17899</x:v>
+        <x:v>16600</x:v>
       </x:c>
       <x:c r="L26" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M26">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N26">
-        <x:v>421000</x:v>
+        <x:v>236200</x:v>
       </x:c>
       <x:c r="O26">
-        <x:v>5499</x:v>
+        <x:v>5100</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:15">
@@ -2036,43 +2036,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C27" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D27" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E27">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F27">
-        <x:v>11601</x:v>
+        <x:v>18500</x:v>
       </x:c>
       <x:c r="G27">
-        <x:v>12300</x:v>
+        <x:v>19401</x:v>
       </x:c>
       <x:c r="H27" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I27">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J27">
-        <x:v>500900</x:v>
+        <x:v>526300</x:v>
       </x:c>
       <x:c r="K27">
-        <x:v>13300</x:v>
+        <x:v>43200</x:v>
       </x:c>
       <x:c r="L27" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M27">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N27">
-        <x:v>500900</x:v>
+        <x:v>526300</x:v>
       </x:c>
       <x:c r="O27">
-        <x:v>52299</x:v>
+        <x:v>5801</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:15">
@@ -2083,43 +2083,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C28" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D28" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E28">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F28">
-        <x:v>18302</x:v>
+        <x:v>14200</x:v>
       </x:c>
       <x:c r="G28">
-        <x:v>17400</x:v>
+        <x:v>22200</x:v>
       </x:c>
       <x:c r="H28" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I28">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J28">
-        <x:v>251800</x:v>
+        <x:v>302300</x:v>
       </x:c>
       <x:c r="K28">
-        <x:v>16901</x:v>
+        <x:v>18199</x:v>
       </x:c>
       <x:c r="L28" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M28">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N28">
-        <x:v>251800</x:v>
+        <x:v>302300</x:v>
       </x:c>
       <x:c r="O28">
-        <x:v>4901</x:v>
+        <x:v>4400</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:15">
@@ -2130,43 +2130,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C29" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D29" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E29">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F29">
-        <x:v>14100</x:v>
+        <x:v>12699</x:v>
       </x:c>
       <x:c r="G29">
-        <x:v>17500</x:v>
+        <x:v>16800</x:v>
       </x:c>
       <x:c r="H29" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I29">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J29">
-        <x:v>346500</x:v>
+        <x:v>138600</x:v>
       </x:c>
       <x:c r="K29">
-        <x:v>16301</x:v>
+        <x:v>12299</x:v>
       </x:c>
       <x:c r="L29" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M29">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N29">
-        <x:v>346500</x:v>
+        <x:v>138600</x:v>
       </x:c>
       <x:c r="O29">
-        <x:v>5100</x:v>
+        <x:v>5500</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:15">
@@ -2177,43 +2177,43 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="C30" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D30" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E30">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="F30">
-        <x:v>13599</x:v>
+        <x:v>14301</x:v>
       </x:c>
       <x:c r="G30">
-        <x:v>16399</x:v>
+        <x:v>20101</x:v>
       </x:c>
       <x:c r="H30" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="I30">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="J30">
-        <x:v>361500</x:v>
+        <x:v>560999</x:v>
       </x:c>
       <x:c r="K30">
-        <x:v>15500</x:v>
+        <x:v>15300</x:v>
       </x:c>
       <x:c r="L30" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="M30">
-        <x:v>1</x:v>
+        <x:v>1.41421356237309</x:v>
       </x:c>
       <x:c r="N30">
-        <x:v>361500</x:v>
+        <x:v>560999</x:v>
       </x:c>
       <x:c r="O30">
-        <x:v>5000</x:v>
+        <x:v>4701</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:15">
@@ -2224,43 +2224,43 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C31" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D31" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D31" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="E31">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="F31">
-        <x:v>211900</x:v>
+        <x:v>27300</x:v>
       </x:c>
       <x:c r="G31">
-        <x:v>65799</x:v>
+        <x:v>36299</x:v>
       </x:c>
       <x:c r="H31" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I31">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="J31">
-        <x:v>469401</x:v>
+        <x:v>426700</x:v>
       </x:c>
       <x:c r="K31">
-        <x:v>14100</x:v>
+        <x:v>14399</x:v>
       </x:c>
       <x:c r="L31" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="M31">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="N31">
-        <x:v>469401</x:v>
+        <x:v>426700</x:v>
       </x:c>
       <x:c r="O31">
-        <x:v>4401</x:v>
+        <x:v>14200</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:15">
@@ -2271,43 +2271,43 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C32" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D32" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D32" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="E32">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="F32">
-        <x:v>26801</x:v>
+        <x:v>27900</x:v>
       </x:c>
       <x:c r="G32">
-        <x:v>33899</x:v>
+        <x:v>45700</x:v>
       </x:c>
       <x:c r="H32" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I32">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="J32">
-        <x:v>432999</x:v>
+        <x:v>498800</x:v>
       </x:c>
       <x:c r="K32">
-        <x:v>15400</x:v>
+        <x:v>15500</x:v>
       </x:c>
       <x:c r="L32" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="M32">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="N32">
-        <x:v>432999</x:v>
+        <x:v>498800</x:v>
       </x:c>
       <x:c r="O32">
-        <x:v>5401</x:v>
+        <x:v>6200</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:15">
@@ -2318,43 +2318,43 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C33" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D33" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D33" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="E33">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="F33">
-        <x:v>17301</x:v>
+        <x:v>25999</x:v>
       </x:c>
       <x:c r="G33">
-        <x:v>22700</x:v>
+        <x:v>32600</x:v>
       </x:c>
       <x:c r="H33" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I33">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="J33">
-        <x:v>343700</x:v>
+        <x:v>653301</x:v>
       </x:c>
       <x:c r="K33">
-        <x:v>41100</x:v>
+        <x:v>16800</x:v>
       </x:c>
       <x:c r="L33" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="M33">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="N33">
-        <x:v>343700</x:v>
+        <x:v>653301</x:v>
       </x:c>
       <x:c r="O33">
-        <x:v>4399</x:v>
+        <x:v>5399</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:15">
@@ -2365,43 +2365,43 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C34" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D34" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D34" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="E34">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="F34">
-        <x:v>29301</x:v>
+        <x:v>26700</x:v>
       </x:c>
       <x:c r="G34">
-        <x:v>35500</x:v>
+        <x:v>35700</x:v>
       </x:c>
       <x:c r="H34" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I34">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="J34">
-        <x:v>308900</x:v>
+        <x:v>325701</x:v>
       </x:c>
       <x:c r="K34">
-        <x:v>13600</x:v>
+        <x:v>14700</x:v>
       </x:c>
       <x:c r="L34" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="M34">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="N34">
-        <x:v>308900</x:v>
+        <x:v>325701</x:v>
       </x:c>
       <x:c r="O34">
-        <x:v>5399</x:v>
+        <x:v>5400</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:15">
@@ -2412,40 +2412,40 @@
         <x:v>80</x:v>
       </x:c>
       <x:c r="C35" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D35" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D35" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="E35">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="F35">
-        <x:v>26699</x:v>
+        <x:v>29303</x:v>
       </x:c>
       <x:c r="G35">
-        <x:v>31700</x:v>
+        <x:v>33399</x:v>
       </x:c>
       <x:c r="H35" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I35">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="J35">
-        <x:v>306400</x:v>
+        <x:v>386400</x:v>
       </x:c>
       <x:c r="K35">
-        <x:v>13001</x:v>
+        <x:v>16600</x:v>
       </x:c>
       <x:c r="L35" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="M35">
-        <x:v>4</x:v>
+        <x:v>4.3588989435406704</x:v>
       </x:c>
       <x:c r="N35">
-        <x:v>306400</x:v>
+        <x:v>386400</x:v>
       </x:c>
       <x:c r="O35">
         <x:v>5000</x:v>
@@ -2459,43 +2459,43 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="C36" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D36" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E36">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="F36">
-        <x:v>37300</x:v>
+        <x:v>29699</x:v>
       </x:c>
       <x:c r="G36">
-        <x:v>41200</x:v>
+        <x:v>40800</x:v>
       </x:c>
       <x:c r="H36" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I36">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="J36">
-        <x:v>1167700</x:v>
+        <x:v>1351000</x:v>
       </x:c>
       <x:c r="K36">
-        <x:v>16700</x:v>
+        <x:v>17101</x:v>
       </x:c>
       <x:c r="L36" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M36">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="N36">
-        <x:v>1167700</x:v>
+        <x:v>1351000</x:v>
       </x:c>
       <x:c r="O36">
-        <x:v>261501</x:v>
+        <x:v>51599</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:15">
@@ -2506,43 +2506,43 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="C37" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D37" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E37">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="F37">
-        <x:v>45799</x:v>
+        <x:v>46604</x:v>
       </x:c>
       <x:c r="G37">
-        <x:v>57599</x:v>
+        <x:v>72800</x:v>
       </x:c>
       <x:c r="H37" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I37">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="J37">
-        <x:v>829099</x:v>
+        <x:v>765600</x:v>
       </x:c>
       <x:c r="K37">
-        <x:v>11799</x:v>
+        <x:v>15400</x:v>
       </x:c>
       <x:c r="L37" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M37">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="N37">
-        <x:v>829099</x:v>
+        <x:v>765600</x:v>
       </x:c>
       <x:c r="O37">
-        <x:v>34601</x:v>
+        <x:v>37201</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:15">
@@ -2553,43 +2553,43 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="C38" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D38" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E38">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="F38">
-        <x:v>46800</x:v>
+        <x:v>30000</x:v>
       </x:c>
       <x:c r="G38">
-        <x:v>60100</x:v>
+        <x:v>43800</x:v>
       </x:c>
       <x:c r="H38" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I38">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="J38">
-        <x:v>836899</x:v>
+        <x:v>869900</x:v>
       </x:c>
       <x:c r="K38">
-        <x:v>11399</x:v>
+        <x:v>19099</x:v>
       </x:c>
       <x:c r="L38" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M38">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="N38">
-        <x:v>836899</x:v>
+        <x:v>869900</x:v>
       </x:c>
       <x:c r="O38">
-        <x:v>31400</x:v>
+        <x:v>36401</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:15">
@@ -2600,43 +2600,43 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="C39" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D39" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E39">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="F39">
-        <x:v>52598</x:v>
+        <x:v>62099</x:v>
       </x:c>
       <x:c r="G39">
-        <x:v>69800</x:v>
+        <x:v>120400</x:v>
       </x:c>
       <x:c r="H39" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I39">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="J39">
-        <x:v>1615601</x:v>
+        <x:v>730900</x:v>
       </x:c>
       <x:c r="K39">
-        <x:v>16900</x:v>
+        <x:v>11599</x:v>
       </x:c>
       <x:c r="L39" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M39">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="N39">
-        <x:v>1615601</x:v>
+        <x:v>730900</x:v>
       </x:c>
       <x:c r="O39">
-        <x:v>391600</x:v>
+        <x:v>36799</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:15">
@@ -2647,43 +2647,43 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="C40" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D40" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E40">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="F40">
-        <x:v>29902</x:v>
+        <x:v>51698</x:v>
       </x:c>
       <x:c r="G40">
-        <x:v>41100</x:v>
+        <x:v>68300</x:v>
       </x:c>
       <x:c r="H40" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="I40">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="J40">
-        <x:v>2090300</x:v>
+        <x:v>859101</x:v>
       </x:c>
       <x:c r="K40">
-        <x:v>16500</x:v>
+        <x:v>17200</x:v>
       </x:c>
       <x:c r="L40" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="M40">
-        <x:v>3</x:v>
+        <x:v>3.1622776601683702</x:v>
       </x:c>
       <x:c r="N40">
-        <x:v>2090300</x:v>
+        <x:v>859101</x:v>
       </x:c>
       <x:c r="O40">
-        <x:v>492500</x:v>
+        <x:v>38601</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:15">
@@ -2694,43 +2694,43 @@
         <x:v>320</x:v>
       </x:c>
       <x:c r="C41" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D41" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E41">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="F41">
-        <x:v>99497</x:v>
+        <x:v>90704</x:v>
       </x:c>
       <x:c r="G41">
-        <x:v>136699</x:v>
+        <x:v>414000</x:v>
       </x:c>
       <x:c r="H41" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I41">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="J41">
-        <x:v>1804300</x:v>
+        <x:v>1755400</x:v>
       </x:c>
       <x:c r="K41">
-        <x:v>16501</x:v>
+        <x:v>17799</x:v>
       </x:c>
       <x:c r="L41" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M41">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="N41">
-        <x:v>1804300</x:v>
+        <x:v>1755400</x:v>
       </x:c>
       <x:c r="O41">
-        <x:v>28000</x:v>
+        <x:v>30700</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:15">
@@ -2741,43 +2741,43 @@
         <x:v>320</x:v>
       </x:c>
       <x:c r="C42" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D42" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E42">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="F42">
-        <x:v>102798</x:v>
+        <x:v>56799</x:v>
       </x:c>
       <x:c r="G42">
-        <x:v>119300</x:v>
+        <x:v>82600</x:v>
       </x:c>
       <x:c r="H42" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I42">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="J42">
-        <x:v>2162800</x:v>
+        <x:v>1916800</x:v>
       </x:c>
       <x:c r="K42">
-        <x:v>17701</x:v>
+        <x:v>17001</x:v>
       </x:c>
       <x:c r="L42" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M42">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="N42">
-        <x:v>2162800</x:v>
+        <x:v>1916800</x:v>
       </x:c>
       <x:c r="O42">
-        <x:v>24000</x:v>
+        <x:v>26700</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:15">
@@ -2788,43 +2788,43 @@
         <x:v>320</x:v>
       </x:c>
       <x:c r="C43" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D43" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E43">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="F43">
-        <x:v>96605</x:v>
+        <x:v>91104</x:v>
       </x:c>
       <x:c r="G43">
-        <x:v>130001</x:v>
+        <x:v>161900</x:v>
       </x:c>
       <x:c r="H43" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I43">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="J43">
-        <x:v>2174200</x:v>
+        <x:v>9176799</x:v>
       </x:c>
       <x:c r="K43">
-        <x:v>18701</x:v>
+        <x:v>18300</x:v>
       </x:c>
       <x:c r="L43" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M43">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="N43">
-        <x:v>2174200</x:v>
+        <x:v>9176799</x:v>
       </x:c>
       <x:c r="O43">
-        <x:v>26300</x:v>
+        <x:v>21600</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:15">
@@ -2835,43 +2835,43 @@
         <x:v>320</x:v>
       </x:c>
       <x:c r="C44" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D44" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E44">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="F44">
-        <x:v>95096</x:v>
+        <x:v>95392</x:v>
       </x:c>
       <x:c r="G44">
-        <x:v>124400</x:v>
+        <x:v>144900</x:v>
       </x:c>
       <x:c r="H44" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I44">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="J44">
-        <x:v>4550301</x:v>
+        <x:v>2342501</x:v>
       </x:c>
       <x:c r="K44">
-        <x:v>20200</x:v>
+        <x:v>18800</x:v>
       </x:c>
       <x:c r="L44" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M44">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="N44">
-        <x:v>4550301</x:v>
+        <x:v>2342501</x:v>
       </x:c>
       <x:c r="O44">
-        <x:v>21500</x:v>
+        <x:v>22400</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:15">
@@ -2882,43 +2882,43 @@
         <x:v>320</x:v>
       </x:c>
       <x:c r="C45" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D45" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E45">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="F45">
-        <x:v>98396</x:v>
+        <x:v>99300</x:v>
       </x:c>
       <x:c r="G45">
-        <x:v>137400</x:v>
+        <x:v>124500</x:v>
       </x:c>
       <x:c r="H45" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I45">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="J45">
-        <x:v>938100</x:v>
+        <x:v>4374899</x:v>
       </x:c>
       <x:c r="K45">
-        <x:v>17999</x:v>
+        <x:v>29500</x:v>
       </x:c>
       <x:c r="L45" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="M45">
-        <x:v>5</x:v>
+        <x:v>5.0990195135927801</x:v>
       </x:c>
       <x:c r="N45">
-        <x:v>938100</x:v>
+        <x:v>4374899</x:v>
       </x:c>
       <x:c r="O45">
-        <x:v>21499</x:v>
+        <x:v>20101</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:15">
@@ -2929,43 +2929,43 @@
         <x:v>640</x:v>
       </x:c>
       <x:c r="C46" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D46" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E46">
         <x:v>3</x:v>
       </x:c>
       <x:c r="F46">
-        <x:v>214196</x:v>
+        <x:v>191704</x:v>
       </x:c>
       <x:c r="G46">
-        <x:v>265700</x:v>
+        <x:v>278699</x:v>
       </x:c>
       <x:c r="H46" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I46">
-        <x:v>8</x:v>
+        <x:v>8.3066238629180695</x:v>
       </x:c>
       <x:c r="J46">
-        <x:v>2583900</x:v>
+        <x:v>2106899</x:v>
       </x:c>
       <x:c r="K46">
-        <x:v>67000</x:v>
+        <x:v>66500</x:v>
       </x:c>
       <x:c r="L46" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M46">
         <x:v>3</x:v>
       </x:c>
       <x:c r="N46">
-        <x:v>2583900</x:v>
+        <x:v>2106899</x:v>
       </x:c>
       <x:c r="O46">
-        <x:v>17900</x:v>
+        <x:v>16200</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:15">
@@ -2976,43 +2976,43 @@
         <x:v>640</x:v>
       </x:c>
       <x:c r="C47" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D47" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E47">
         <x:v>3</x:v>
       </x:c>
       <x:c r="F47">
-        <x:v>184903</x:v>
+        <x:v>193191</x:v>
       </x:c>
       <x:c r="G47">
-        <x:v>3170901</x:v>
+        <x:v>342000</x:v>
       </x:c>
       <x:c r="H47" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I47">
-        <x:v>8</x:v>
+        <x:v>8.3066238629180695</x:v>
       </x:c>
       <x:c r="J47">
-        <x:v>1903599</x:v>
+        <x:v>2299599</x:v>
       </x:c>
       <x:c r="K47">
-        <x:v>18899</x:v>
+        <x:v>19100</x:v>
       </x:c>
       <x:c r="L47" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M47">
         <x:v>3</x:v>
       </x:c>
       <x:c r="N47">
-        <x:v>1903599</x:v>
+        <x:v>2299599</x:v>
       </x:c>
       <x:c r="O47">
-        <x:v>14600</x:v>
+        <x:v>17800</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:15">
@@ -3023,43 +3023,43 @@
         <x:v>640</x:v>
       </x:c>
       <x:c r="C48" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D48" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E48">
         <x:v>3</x:v>
       </x:c>
       <x:c r="F48">
-        <x:v>185796</x:v>
+        <x:v>195397</x:v>
       </x:c>
       <x:c r="G48">
-        <x:v>336600</x:v>
+        <x:v>292900</x:v>
       </x:c>
       <x:c r="H48" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I48">
-        <x:v>8</x:v>
+        <x:v>8.3066238629180695</x:v>
       </x:c>
       <x:c r="J48">
-        <x:v>1951500</x:v>
+        <x:v>2167301</x:v>
       </x:c>
       <x:c r="K48">
-        <x:v>17901</x:v>
+        <x:v>19701</x:v>
       </x:c>
       <x:c r="L48" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M48">
         <x:v>3</x:v>
       </x:c>
       <x:c r="N48">
-        <x:v>1951500</x:v>
+        <x:v>2167301</x:v>
       </x:c>
       <x:c r="O48">
-        <x:v>17000</x:v>
+        <x:v>17600</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:15">
@@ -3070,43 +3070,43 @@
         <x:v>640</x:v>
       </x:c>
       <x:c r="C49" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D49" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E49">
         <x:v>3</x:v>
       </x:c>
       <x:c r="F49">
-        <x:v>203806</x:v>
+        <x:v>195414</x:v>
       </x:c>
       <x:c r="G49">
-        <x:v>1571500</x:v>
+        <x:v>140100</x:v>
       </x:c>
       <x:c r="H49" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I49">
-        <x:v>8</x:v>
+        <x:v>8.3066238629180695</x:v>
       </x:c>
       <x:c r="J49">
-        <x:v>7430700</x:v>
+        <x:v>2384800</x:v>
       </x:c>
       <x:c r="K49">
-        <x:v>20200</x:v>
+        <x:v>22501</x:v>
       </x:c>
       <x:c r="L49" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M49">
         <x:v>3</x:v>
       </x:c>
       <x:c r="N49">
-        <x:v>7430700</x:v>
+        <x:v>2384800</x:v>
       </x:c>
       <x:c r="O49">
-        <x:v>15800</x:v>
+        <x:v>17700</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:15">
@@ -3117,43 +3117,43 @@
         <x:v>640</x:v>
       </x:c>
       <x:c r="C50" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D50" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E50">
         <x:v>3</x:v>
       </x:c>
       <x:c r="F50">
-        <x:v>261296</x:v>
+        <x:v>208792</x:v>
       </x:c>
       <x:c r="G50">
-        <x:v>346299</x:v>
+        <x:v>136400</x:v>
       </x:c>
       <x:c r="H50" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I50">
-        <x:v>8</x:v>
+        <x:v>8.3066238629180695</x:v>
       </x:c>
       <x:c r="J50">
-        <x:v>2113400</x:v>
+        <x:v>4888800</x:v>
       </x:c>
       <x:c r="K50">
-        <x:v>21500</x:v>
+        <x:v>277799</x:v>
       </x:c>
       <x:c r="L50" t="s">
-        <x:v>6</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="M50">
         <x:v>3</x:v>
       </x:c>
       <x:c r="N50">
-        <x:v>2113400</x:v>
+        <x:v>4888800</x:v>
       </x:c>
       <x:c r="O50">
-        <x:v>18300</x:v>
+        <x:v>20500</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:15">
@@ -3164,43 +3164,43 @@
         <x:v>1280</x:v>
       </x:c>
       <x:c r="C51" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D51" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E51">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="F51">
-        <x:v>1323705</x:v>
+        <x:v>520697</x:v>
       </x:c>
       <x:c r="G51">
-        <x:v>354300</x:v>
+        <x:v>283599</x:v>
       </x:c>
       <x:c r="H51" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I51">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="J51">
-        <x:v>4430300</x:v>
+        <x:v>5637800</x:v>
       </x:c>
       <x:c r="K51">
-        <x:v>25800</x:v>
+        <x:v>22800</x:v>
       </x:c>
       <x:c r="L51" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="M51">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="N51">
-        <x:v>4430300</x:v>
+        <x:v>5637800</x:v>
       </x:c>
       <x:c r="O51">
-        <x:v>13201</x:v>
+        <x:v>12801</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:15">
@@ -3211,43 +3211,43 @@
         <x:v>1280</x:v>
       </x:c>
       <x:c r="C52" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D52" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E52">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="F52">
-        <x:v>353997</x:v>
+        <x:v>1185799</x:v>
       </x:c>
       <x:c r="G52">
-        <x:v>312600</x:v>
+        <x:v>612300</x:v>
       </x:c>
       <x:c r="H52" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I52">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="J52">
-        <x:v>4528499</x:v>
+        <x:v>4800800</x:v>
       </x:c>
       <x:c r="K52">
-        <x:v>25099</x:v>
+        <x:v>23401</x:v>
       </x:c>
       <x:c r="L52" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="M52">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="N52">
-        <x:v>4528499</x:v>
+        <x:v>4800800</x:v>
       </x:c>
       <x:c r="O52">
-        <x:v>12700</x:v>
+        <x:v>12901</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:15">
@@ -3258,43 +3258,43 @@
         <x:v>1280</x:v>
       </x:c>
       <x:c r="C53" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D53" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E53">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="F53">
-        <x:v>351205</x:v>
+        <x:v>377994</x:v>
       </x:c>
       <x:c r="G53">
-        <x:v>336100</x:v>
+        <x:v>3841999</x:v>
       </x:c>
       <x:c r="H53" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I53">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="J53">
-        <x:v>7593200</x:v>
+        <x:v>4215399</x:v>
       </x:c>
       <x:c r="K53">
-        <x:v>48900</x:v>
+        <x:v>24899</x:v>
       </x:c>
       <x:c r="L53" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="M53">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="N53">
-        <x:v>7593200</x:v>
+        <x:v>4215399</x:v>
       </x:c>
       <x:c r="O53">
-        <x:v>13300</x:v>
+        <x:v>118301</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:15">
@@ -3305,43 +3305,43 @@
         <x:v>1280</x:v>
       </x:c>
       <x:c r="C54" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D54" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E54">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="F54">
-        <x:v>307396</x:v>
+        <x:v>345895</x:v>
       </x:c>
       <x:c r="G54">
-        <x:v>309800</x:v>
+        <x:v>287199</x:v>
       </x:c>
       <x:c r="H54" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I54">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="J54">
-        <x:v>6139799</x:v>
+        <x:v>4325401</x:v>
       </x:c>
       <x:c r="K54">
-        <x:v>23000</x:v>
+        <x:v>24800</x:v>
       </x:c>
       <x:c r="L54" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="M54">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="N54">
-        <x:v>6139799</x:v>
+        <x:v>4325401</x:v>
       </x:c>
       <x:c r="O54">
-        <x:v>12301</x:v>
+        <x:v>12000</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:15">
@@ -3352,43 +3352,43 @@
         <x:v>1280</x:v>
       </x:c>
       <x:c r="C55" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D55" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E55">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="F55">
-        <x:v>367594</x:v>
+        <x:v>342502</x:v>
       </x:c>
       <x:c r="G55">
-        <x:v>301999</x:v>
+        <x:v>283600</x:v>
       </x:c>
       <x:c r="H55" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I55">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="J55">
-        <x:v>4167301</x:v>
+        <x:v>8561600</x:v>
       </x:c>
       <x:c r="K55">
-        <x:v>21200</x:v>
+        <x:v>25600</x:v>
       </x:c>
       <x:c r="L55" t="s">
-        <x:v>4</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="M55">
-        <x:v>3</x:v>
+        <x:v>3.4641016151377499</x:v>
       </x:c>
       <x:c r="N55">
-        <x:v>4167301</x:v>
+        <x:v>8561600</x:v>
       </x:c>
       <x:c r="O55">
-        <x:v>12600</x:v>
+        <x:v>14000</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:15">
@@ -3399,43 +3399,43 @@
         <x:v>2560</x:v>
       </x:c>
       <x:c r="C56" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D56" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E56">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="F56">
-        <x:v>709996</x:v>
+        <x:v>692385</x:v>
       </x:c>
       <x:c r="G56">
-        <x:v>1127200</x:v>
+        <x:v>591100</x:v>
       </x:c>
       <x:c r="H56" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I56">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="J56">
-        <x:v>9941101</x:v>
+        <x:v>4.5825756949558398</x:v>
+      </x:c>
+      <x:c r="J56" s="1">
+        <x:v>13634900</x:v>
       </x:c>
       <x:c r="K56">
-        <x:v>23600</x:v>
+        <x:v>26600</x:v>
       </x:c>
       <x:c r="L56" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M56">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N56">
-        <x:v>9941101</x:v>
+        <x:v>4.5825756949558398</x:v>
+      </x:c>
+      <x:c r="N56" s="1">
+        <x:v>13634900</x:v>
       </x:c>
       <x:c r="O56">
-        <x:v>9000</x:v>
+        <x:v>8799</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:15">
@@ -3446,43 +3446,43 @@
         <x:v>2560</x:v>
       </x:c>
       <x:c r="C57" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D57" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E57">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="F57">
-        <x:v>641597</x:v>
+        <x:v>683398</x:v>
       </x:c>
       <x:c r="G57">
-        <x:v>626300</x:v>
+        <x:v>548900</x:v>
       </x:c>
       <x:c r="H57" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I57">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="J57" s="1">
-        <x:v>12258399</x:v>
+        <x:v>12169600</x:v>
       </x:c>
       <x:c r="K57">
         <x:v>26700</x:v>
       </x:c>
       <x:c r="L57" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M57">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="N57" s="1">
-        <x:v>12258399</x:v>
+        <x:v>12169600</x:v>
       </x:c>
       <x:c r="O57">
-        <x:v>8500</x:v>
+        <x:v>18000</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:15">
@@ -3493,40 +3493,40 @@
         <x:v>2560</x:v>
       </x:c>
       <x:c r="C58" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D58" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E58">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="F58">
-        <x:v>659206</x:v>
+        <x:v>669497</x:v>
       </x:c>
       <x:c r="G58">
-        <x:v>757101</x:v>
+        <x:v>614800</x:v>
       </x:c>
       <x:c r="H58" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I58">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="J58" s="1">
-        <x:v>13398100</x:v>
+        <x:v>12289000</x:v>
       </x:c>
       <x:c r="K58">
-        <x:v>34201</x:v>
+        <x:v>24900</x:v>
       </x:c>
       <x:c r="L58" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M58">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="N58" s="1">
-        <x:v>13398100</x:v>
+        <x:v>12289000</x:v>
       </x:c>
       <x:c r="O58">
         <x:v>8601</x:v>
@@ -3540,43 +3540,43 @@
         <x:v>2560</x:v>
       </x:c>
       <x:c r="C59" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D59" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E59">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="F59">
-        <x:v>654096</x:v>
+        <x:v>683987</x:v>
       </x:c>
       <x:c r="G59">
-        <x:v>616999</x:v>
+        <x:v>560500</x:v>
       </x:c>
       <x:c r="H59" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I59">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="J59" s="1">
-        <x:v>12928400</x:v>
+        <x:v>4.5825756949558398</x:v>
+      </x:c>
+      <x:c r="J59">
+        <x:v>9226701</x:v>
       </x:c>
       <x:c r="K59">
-        <x:v>25900</x:v>
+        <x:v>1063301</x:v>
       </x:c>
       <x:c r="L59" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M59">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N59" s="1">
-        <x:v>12928400</x:v>
+        <x:v>4.5825756949558398</x:v>
+      </x:c>
+      <x:c r="N59">
+        <x:v>9226701</x:v>
       </x:c>
       <x:c r="O59">
-        <x:v>8900</x:v>
+        <x:v>9701</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:15">
@@ -3587,43 +3587,43 @@
         <x:v>2560</x:v>
       </x:c>
       <x:c r="C60" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D60" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E60">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="F60">
-        <x:v>690299</x:v>
+        <x:v>603797</x:v>
       </x:c>
       <x:c r="G60">
-        <x:v>703700</x:v>
+        <x:v>558800</x:v>
       </x:c>
       <x:c r="H60" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="I60">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="J60" s="1">
-        <x:v>11626000</x:v>
+        <x:v>10767200</x:v>
       </x:c>
       <x:c r="K60">
-        <x:v>27800</x:v>
+        <x:v>35201</x:v>
       </x:c>
       <x:c r="L60" t="s">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="M60">
-        <x:v>4</x:v>
+        <x:v>4.5825756949558398</x:v>
       </x:c>
       <x:c r="N60" s="1">
-        <x:v>11626000</x:v>
+        <x:v>10767200</x:v>
       </x:c>
       <x:c r="O60">
-        <x:v>17901</x:v>
+        <x:v>22700</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>